<commit_message>
schema fixes, still cant catch uNAme
</commit_message>
<xml_diff>
--- a/eligible_participants.xlsx
+++ b/eligible_participants.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -471,9 +471,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>923866421811879967</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implemented xlsx export, help  and about command
</commit_message>
<xml_diff>
--- a/eligible_participants.xlsx
+++ b/eligible_participants.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -420,6 +420,9 @@
       <c r="A2" t="str">
         <v>923866421811879967</v>
       </c>
+      <c r="B2" t="str">
+        <v>saalim192</v>
+      </c>
       <c r="C2" t="str">
         <v>Twitter</v>
       </c>
@@ -429,62 +432,21 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>923866421811879967</v>
+        <v>957228261610496001</v>
+      </c>
+      <c r="B3" t="str">
+        <v>faizanr7</v>
       </c>
       <c r="C3" t="str">
-        <v>Unknown</v>
+        <v>Twitter</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>923866421811879967</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Unknown</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>923866421811879967</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Unknown</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>923866421811879967</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Unknown</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>923866421811879967</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Unknown</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>